<commit_message>
- Fix upload excel for holiday
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/Perak Public Holiday 2021.xlsx
+++ b/src/main/resources/templates/excel/Perak Public Holiday 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win 10\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRYAN TAN\IdeaProjects\CWSS-backend\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40174476-B13F-4999-BF4C-E9A57F0042B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A560010-71D1-4A87-AC49-0A0ACA26E739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB3C7BA9-9D24-4736-9EB5-443F6AB679D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{EB3C7BA9-9D24-4736-9EB5-443F6AB679D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>New Year 2021</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Thaipusam</t>
   </si>
@@ -45,27 +42,12 @@
     <t>Nuzul Al-Quran</t>
   </si>
   <si>
-    <t>Birthday of His Royal Highness The Sultan Of Perak</t>
-  </si>
-  <si>
     <t>Chinese New Year</t>
   </si>
   <si>
     <t>Labour Day</t>
   </si>
   <si>
-    <t>Hari Raya Puasa</t>
-  </si>
-  <si>
-    <t>Wesak</t>
-  </si>
-  <si>
-    <t>Birthday Of His Majesty The Yang di-Pertuan Agong</t>
-  </si>
-  <si>
-    <t>Hari Raya Qurban</t>
-  </si>
-  <si>
     <t>Awal Muharram</t>
   </si>
   <si>
@@ -88,6 +70,48 @@
   </si>
   <si>
     <t>HOLIDAY_DATE</t>
+  </si>
+  <si>
+    <t>New Year's Day</t>
+  </si>
+  <si>
+    <t>Chinese New Year Holiday</t>
+  </si>
+  <si>
+    <t>Labour Day Holiday</t>
+  </si>
+  <si>
+    <t>Hari Raya Aidilfitri</t>
+  </si>
+  <si>
+    <t>Hari Raya Aidilfitri Holiday</t>
+  </si>
+  <si>
+    <t>Wesak Day</t>
+  </si>
+  <si>
+    <t>Wesak Day Holiday</t>
+  </si>
+  <si>
+    <t>Agong's Birthday</t>
+  </si>
+  <si>
+    <t>Hari Raya Haji</t>
+  </si>
+  <si>
+    <t>Hari Raya Haji Holiday</t>
+  </si>
+  <si>
+    <t>Prophet Muhammad's Birthday Holiday</t>
+  </si>
+  <si>
+    <t>Sultan of Perak's Birthday</t>
+  </si>
+  <si>
+    <t>Christmas Holiday</t>
+  </si>
+  <si>
+    <t>YEAR</t>
   </si>
 </sst>
 </file>
@@ -440,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB142C7-98CE-45D9-9782-611A057D14D6}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,156 +476,269 @@
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44562</v>
+      </c>
+      <c r="C2">
+        <v>2022</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>44197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
       <c r="B3" s="1">
-        <v>44224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44579</v>
+      </c>
+      <c r="C3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>44315</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44593</v>
+      </c>
+      <c r="C4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44594</v>
+      </c>
+      <c r="C5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44670</v>
+      </c>
+      <c r="C6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>44505</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" s="1">
+        <v>44682</v>
+      </c>
+      <c r="C7">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44683</v>
+      </c>
+      <c r="C8">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44684</v>
+      </c>
+      <c r="C9">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44685</v>
+      </c>
+      <c r="C10">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44696</v>
+      </c>
+      <c r="C11">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44697</v>
+      </c>
+      <c r="C12">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44718</v>
+      </c>
+      <c r="C13">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44752</v>
+      </c>
+      <c r="C14">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44753</v>
+      </c>
+      <c r="C15">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>44239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44240</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B16" s="1">
+        <v>44772</v>
+      </c>
+      <c r="C16">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
-        <v>44317</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B17" s="1">
+        <v>44804</v>
+      </c>
+      <c r="C17">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1">
-        <v>44329</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1">
-        <v>44330</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B18" s="1">
+        <v>44820</v>
+      </c>
+      <c r="C18">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
-        <v>44342</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B19" s="1">
+        <v>44843</v>
+      </c>
+      <c r="C19">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44844</v>
+      </c>
+      <c r="C20">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1">
-        <v>44354</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B21" s="1">
+        <v>44858</v>
+      </c>
+      <c r="C21">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44869</v>
+      </c>
+      <c r="C22">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1">
-        <v>44397</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44418</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1">
-        <v>44439</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1">
-        <v>44455</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1">
-        <v>44488</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="1">
-        <v>44504</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1">
-        <v>44555</v>
+      <c r="B23" s="1">
+        <v>44920</v>
+      </c>
+      <c r="C23">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44921</v>
+      </c>
+      <c r="C24">
+        <v>2022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Allow admin to manage holiday
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/Perak Public Holiday 2021.xlsx
+++ b/src/main/resources/templates/excel/Perak Public Holiday 2021.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRYAN TAN\IdeaProjects\CWSS-backend\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A560010-71D1-4A87-AC49-0A0ACA26E739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336892B8-7F14-4C8A-A88F-60964C22264F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{EB3C7BA9-9D24-4736-9EB5-443F6AB679D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{EB3C7BA9-9D24-4736-9EB5-443F6AB679D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Instruction" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Thaipusam</t>
   </si>
@@ -112,14 +113,30 @@
   </si>
   <si>
     <t>YEAR</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>1. Please follow the exact template like Sheet1. Otherwise there'll be issue when adding holidays.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,9 +164,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB142C7-98CE-45D9-9782-611A057D14D6}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,4 +763,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C463ED1-0C2E-4379-B00A-EE19A658D6B4}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>